<commit_message>
optimized folder structure and added comments
</commit_message>
<xml_diff>
--- a/lead_data.xlsx
+++ b/lead_data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="91">
   <si>
     <t>id</t>
   </si>
@@ -44,12 +44,6 @@
     <t>lead_category</t>
   </si>
   <si>
-    <t>technology</t>
-  </si>
-  <si>
-    <t>complexity</t>
-  </si>
-  <si>
     <t>created_at</t>
   </si>
   <si>
@@ -116,6 +110,12 @@
     <t>A company page</t>
   </si>
   <si>
+    <t>Website Inquiry</t>
+  </si>
+  <si>
+    <t>Linkedin</t>
+  </si>
+  <si>
     <t>New</t>
   </si>
   <si>
@@ -167,6 +167,15 @@
     <t xml:space="preserve">test@xyz.com	</t>
   </si>
   <si>
+    <t>testa@gmail.com</t>
+  </si>
+  <si>
+    <t>john.doe@company.com</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
     <t>Interested in CRM integration</t>
   </si>
   <si>
@@ -194,6 +203,15 @@
     <t>ui dev</t>
   </si>
   <si>
+    <t>Agent ai application</t>
+  </si>
+  <si>
+    <t>CRM application</t>
+  </si>
+  <si>
+    <t>An agentic ai application</t>
+  </si>
+  <si>
     <t>2024-02-01</t>
   </si>
   <si>
@@ -212,6 +230,9 @@
     <t>2025-02-09</t>
   </si>
   <si>
+    <t>2025-02-10</t>
+  </si>
+  <si>
     <t>Software</t>
   </si>
   <si>
@@ -230,10 +251,19 @@
     <t>Saas</t>
   </si>
   <si>
+    <t>AI/ML</t>
+  </si>
+  <si>
     <t>Cold Lead</t>
   </si>
   <si>
     <t>Unbound Lead</t>
+  </si>
+  <si>
+    <t>High-value lead</t>
+  </si>
+  <si>
+    <t>Sales</t>
   </si>
   <si>
     <t>status(qualified_status)</t>
@@ -619,13 +649,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,19 +689,13 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -683,27 +707,27 @@
         <v>42</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" s="2">
+        <v>72</v>
+      </c>
+      <c r="J2" s="2">
         <v>45697.62820799769</v>
       </c>
-      <c r="M2" s="2">
-        <v>45697.628208125</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="K2" s="2">
+        <v>45698.0393449537</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -715,27 +739,27 @@
         <v>43</v>
       </c>
       <c r="F3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
-      </c>
-      <c r="L3" s="2">
+        <v>73</v>
+      </c>
+      <c r="J3" s="2">
         <v>45697.62836686343</v>
       </c>
-      <c r="M3" s="2">
-        <v>45697.628366875</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="K3" s="2">
+        <v>45698.04606594907</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -747,27 +771,27 @@
         <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
-      </c>
-      <c r="L4" s="2">
+        <v>74</v>
+      </c>
+      <c r="J4" s="2">
         <v>45697.62852407408</v>
       </c>
-      <c r="M4" s="2">
+      <c r="K4" s="2">
         <v>45697.62852407408</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
         <v>36</v>
@@ -779,27 +803,27 @@
         <v>45</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="2">
+        <v>75</v>
+      </c>
+      <c r="J5" s="2">
         <v>45697.62866636574</v>
       </c>
-      <c r="M5" s="2">
+      <c r="K5" s="2">
         <v>45697.62866636574</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -811,27 +835,27 @@
         <v>46</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" s="2">
+        <v>76</v>
+      </c>
+      <c r="J6" s="2">
         <v>45697.62883305555</v>
       </c>
-      <c r="M6" s="2">
+      <c r="K6" s="2">
         <v>45697.62883305555</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>33</v>
@@ -843,27 +867,27 @@
         <v>42</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" s="2">
+        <v>72</v>
+      </c>
+      <c r="J7" s="2">
         <v>45697.66256271991</v>
       </c>
-      <c r="M7" s="2">
+      <c r="K7" s="2">
         <v>45697.66256276621</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>34</v>
@@ -875,27 +899,27 @@
         <v>43</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
-      </c>
-      <c r="L8" s="2">
+        <v>73</v>
+      </c>
+      <c r="J8" s="2">
         <v>45697.66270547454</v>
       </c>
-      <c r="M8" s="2">
+      <c r="K8" s="2">
         <v>45697.66270548611</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
@@ -907,27 +931,27 @@
         <v>42</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H9" t="s">
-        <v>65</v>
-      </c>
-      <c r="L9" s="2">
+        <v>72</v>
+      </c>
+      <c r="J9" s="2">
         <v>45697.66566469907</v>
       </c>
-      <c r="M9" s="2">
+      <c r="K9" s="2">
         <v>45697.66566469907</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -939,27 +963,27 @@
         <v>43</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
-      </c>
-      <c r="L10" s="2">
+        <v>73</v>
+      </c>
+      <c r="J10" s="2">
         <v>45697.66582216435</v>
       </c>
-      <c r="M10" s="2">
+      <c r="K10" s="2">
         <v>45697.66582216435</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
@@ -971,27 +995,27 @@
         <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>65</v>
-      </c>
-      <c r="L11" s="2">
+        <v>72</v>
+      </c>
+      <c r="J11" s="2">
         <v>45697.67415298611</v>
       </c>
-      <c r="M11" s="2">
+      <c r="K11" s="2">
         <v>45697.67415298611</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -1003,27 +1027,27 @@
         <v>43</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G12" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>66</v>
-      </c>
-      <c r="L12" s="2">
+        <v>73</v>
+      </c>
+      <c r="J12" s="2">
         <v>45697.67428417824</v>
       </c>
-      <c r="M12" s="2">
+      <c r="K12" s="2">
         <v>45697.67428418982</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
@@ -1035,27 +1059,27 @@
         <v>42</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>65</v>
-      </c>
-      <c r="L13" s="2">
+        <v>72</v>
+      </c>
+      <c r="J13" s="2">
         <v>45697.67603481482</v>
       </c>
-      <c r="M13" s="2">
+      <c r="K13" s="2">
         <v>45697.67603481482</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
         <v>34</v>
@@ -1067,27 +1091,27 @@
         <v>43</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
-      </c>
-      <c r="L14" s="2">
+        <v>73</v>
+      </c>
+      <c r="J14" s="2">
         <v>45697.67616851852</v>
       </c>
-      <c r="M14" s="2">
+      <c r="K14" s="2">
         <v>45697.6761685301</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C15" t="s">
         <v>33</v>
@@ -1099,27 +1123,27 @@
         <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
-      </c>
-      <c r="L15" s="2">
+        <v>72</v>
+      </c>
+      <c r="J15" s="2">
         <v>45697.67684298611</v>
       </c>
-      <c r="M15" s="2">
+      <c r="K15" s="2">
         <v>45697.67684298611</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
@@ -1131,27 +1155,27 @@
         <v>43</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G16" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
-      </c>
-      <c r="L16" s="2">
+        <v>73</v>
+      </c>
+      <c r="J16" s="2">
         <v>45697.67698494213</v>
       </c>
-      <c r="M16" s="2">
+      <c r="K16" s="2">
         <v>45697.67698494213</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
         <v>33</v>
@@ -1163,27 +1187,27 @@
         <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H17" t="s">
-        <v>65</v>
-      </c>
-      <c r="L17" s="2">
+        <v>72</v>
+      </c>
+      <c r="J17" s="2">
         <v>45697.68212028936</v>
       </c>
-      <c r="M17" s="2">
-        <v>45697.68212047454</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="K17" s="2">
+        <v>45698.12099792824</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C18" t="s">
         <v>34</v>
@@ -1195,27 +1219,27 @@
         <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H18" t="s">
-        <v>66</v>
-      </c>
-      <c r="L18" s="2">
+        <v>73</v>
+      </c>
+      <c r="J18" s="2">
         <v>45697.68226564815</v>
       </c>
-      <c r="M18" s="2">
+      <c r="K18" s="2">
         <v>45697.68226565972</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
         <v>33</v>
@@ -1227,27 +1251,27 @@
         <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H19" t="s">
-        <v>65</v>
-      </c>
-      <c r="L19" s="2">
+        <v>72</v>
+      </c>
+      <c r="J19" s="2">
         <v>45697.68433324074</v>
       </c>
-      <c r="M19" s="2">
+      <c r="K19" s="2">
         <v>45697.68433324074</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>33</v>
@@ -1259,27 +1283,27 @@
         <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G20" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H20" t="s">
-        <v>65</v>
-      </c>
-      <c r="L20" s="2">
+        <v>72</v>
+      </c>
+      <c r="J20" s="2">
         <v>45697.68575626158</v>
       </c>
-      <c r="M20" s="2">
+      <c r="K20" s="2">
         <v>45697.68575626158</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
@@ -1291,27 +1315,27 @@
         <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G21" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H21" t="s">
-        <v>65</v>
-      </c>
-      <c r="L21" s="2">
+        <v>72</v>
+      </c>
+      <c r="J21" s="2">
         <v>45697.68737824074</v>
       </c>
-      <c r="M21" s="2">
+      <c r="K21" s="2">
         <v>45697.68737824074</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
@@ -1323,27 +1347,27 @@
         <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G22" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H22" t="s">
-        <v>65</v>
-      </c>
-      <c r="L22" s="2">
+        <v>72</v>
+      </c>
+      <c r="J22" s="2">
         <v>45697.6950943287</v>
       </c>
-      <c r="M22" s="2">
+      <c r="K22" s="2">
         <v>45697.69509435185</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
@@ -1355,27 +1379,27 @@
         <v>48</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G23" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H23" t="s">
-        <v>65</v>
-      </c>
-      <c r="L23" s="2">
+        <v>72</v>
+      </c>
+      <c r="J23" s="2">
         <v>45697.69773737268</v>
       </c>
-      <c r="M23" s="2">
+      <c r="K23" s="2">
         <v>45697.69773737268</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
@@ -1387,27 +1411,27 @@
         <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G24" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H24" t="s">
-        <v>65</v>
-      </c>
-      <c r="L24" s="2">
+        <v>72</v>
+      </c>
+      <c r="J24" s="2">
         <v>45697.70470497685</v>
       </c>
-      <c r="M24" s="2">
+      <c r="K24" s="2">
         <v>45697.70470498843</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
@@ -1419,27 +1443,27 @@
         <v>48</v>
       </c>
       <c r="F25" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G25" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H25" t="s">
-        <v>65</v>
-      </c>
-      <c r="L25" s="2">
+        <v>72</v>
+      </c>
+      <c r="J25" s="2">
         <v>45697.70996232639</v>
       </c>
-      <c r="M25" s="2">
+      <c r="K25" s="2">
         <v>45697.70996232639</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
         <v>35</v>
@@ -1451,27 +1475,27 @@
         <v>48</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G26" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H26" t="s">
-        <v>65</v>
-      </c>
-      <c r="L26" s="2">
+        <v>72</v>
+      </c>
+      <c r="J26" s="2">
         <v>45697.71525491899</v>
       </c>
-      <c r="M26" s="2">
-        <v>45697.71525501157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="K26" s="2">
+        <v>45698.07656145834</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
@@ -1483,27 +1507,27 @@
         <v>48</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G27" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H27" t="s">
-        <v>65</v>
-      </c>
-      <c r="L27" s="2">
+        <v>72</v>
+      </c>
+      <c r="J27" s="2">
         <v>45697.72439947916</v>
       </c>
-      <c r="M27" s="2">
+      <c r="K27" s="2">
         <v>45697.72439947916</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
@@ -1515,27 +1539,27 @@
         <v>48</v>
       </c>
       <c r="F28" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G28" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H28" t="s">
-        <v>65</v>
-      </c>
-      <c r="L28" s="2">
+        <v>72</v>
+      </c>
+      <c r="J28" s="2">
         <v>45697.72887666667</v>
       </c>
-      <c r="M28" s="2">
+      <c r="K28" s="2">
         <v>45697.72887666667</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
@@ -1547,27 +1571,27 @@
         <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G29" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H29" t="s">
-        <v>65</v>
-      </c>
-      <c r="L29" s="2">
+        <v>72</v>
+      </c>
+      <c r="J29" s="2">
         <v>45697.73009409722</v>
       </c>
-      <c r="M29" s="2">
+      <c r="K29" s="2">
         <v>45697.73009409722</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
@@ -1579,27 +1603,27 @@
         <v>48</v>
       </c>
       <c r="F30" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="G30" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H30" t="s">
-        <v>65</v>
-      </c>
-      <c r="L30" s="2">
+        <v>72</v>
+      </c>
+      <c r="J30" s="2">
         <v>45697.73256555555</v>
       </c>
-      <c r="M30" s="2">
+      <c r="K30" s="2">
         <v>45697.73256555555</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
         <v>33</v>
@@ -1611,27 +1635,27 @@
         <v>42</v>
       </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G31" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H31" t="s">
-        <v>65</v>
-      </c>
-      <c r="L31" s="2">
+        <v>72</v>
+      </c>
+      <c r="J31" s="2">
         <v>45697.73693395833</v>
       </c>
-      <c r="M31" s="2">
+      <c r="K31" s="2">
         <v>45697.73693395833</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
@@ -1643,27 +1667,27 @@
         <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G32" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H32" t="s">
-        <v>66</v>
-      </c>
-      <c r="L32" s="2">
+        <v>73</v>
+      </c>
+      <c r="J32" s="2">
         <v>45697.73704618055</v>
       </c>
-      <c r="M32" s="2">
+      <c r="K32" s="2">
         <v>45697.73704618055</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
         <v>33</v>
@@ -1675,27 +1699,27 @@
         <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H33" t="s">
-        <v>65</v>
-      </c>
-      <c r="L33" s="2">
+        <v>72</v>
+      </c>
+      <c r="J33" s="2">
         <v>45697.75116141204</v>
       </c>
-      <c r="M33" s="2">
+      <c r="K33" s="2">
         <v>45697.75116153935</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -1707,27 +1731,27 @@
         <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G34" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H34" t="s">
-        <v>66</v>
-      </c>
-      <c r="L34" s="2">
+        <v>73</v>
+      </c>
+      <c r="J34" s="2">
         <v>45697.75128466435</v>
       </c>
-      <c r="M34" s="2">
+      <c r="K34" s="2">
         <v>45697.75128466435</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
         <v>33</v>
@@ -1739,27 +1763,27 @@
         <v>42</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G35" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H35" t="s">
-        <v>65</v>
-      </c>
-      <c r="L35" s="2">
+        <v>72</v>
+      </c>
+      <c r="J35" s="2">
         <v>45697.76037167824</v>
       </c>
-      <c r="M35" s="2">
+      <c r="K35" s="2">
         <v>45697.76037167824</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
         <v>35</v>
@@ -1771,27 +1795,27 @@
         <v>43</v>
       </c>
       <c r="F36" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G36" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H36" t="s">
-        <v>70</v>
-      </c>
-      <c r="L36" s="2">
+        <v>77</v>
+      </c>
+      <c r="J36" s="2">
         <v>45697.76049094908</v>
       </c>
-      <c r="M36" s="2">
+      <c r="K36" s="2">
         <v>45697.76049094908</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
         <v>33</v>
@@ -1803,27 +1827,27 @@
         <v>42</v>
       </c>
       <c r="F37" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G37" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H37" t="s">
-        <v>65</v>
-      </c>
-      <c r="L37" s="2">
+        <v>72</v>
+      </c>
+      <c r="J37" s="2">
         <v>45697.76292693287</v>
       </c>
-      <c r="M37" s="2">
+      <c r="K37" s="2">
         <v>45697.76292694444</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
         <v>35</v>
@@ -1835,27 +1859,27 @@
         <v>43</v>
       </c>
       <c r="F38" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G38" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H38" t="s">
-        <v>70</v>
-      </c>
-      <c r="L38" s="2">
+        <v>77</v>
+      </c>
+      <c r="J38" s="2">
         <v>45697.76303063658</v>
       </c>
-      <c r="M38" s="2">
+      <c r="K38" s="2">
         <v>45697.76303064815</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
@@ -1867,27 +1891,27 @@
         <v>42</v>
       </c>
       <c r="F39" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G39" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H39" t="s">
-        <v>65</v>
-      </c>
-      <c r="L39" s="2">
+        <v>72</v>
+      </c>
+      <c r="J39" s="2">
         <v>45697.77118141203</v>
       </c>
-      <c r="M39" s="2">
+      <c r="K39" s="2">
         <v>45697.77119032407</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C40" t="s">
         <v>35</v>
@@ -1899,27 +1923,27 @@
         <v>43</v>
       </c>
       <c r="F40" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G40" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="H40" t="s">
-        <v>70</v>
-      </c>
-      <c r="L40" s="2">
+        <v>77</v>
+      </c>
+      <c r="J40" s="2">
         <v>45697.77134046296</v>
       </c>
-      <c r="M40" s="2">
+      <c r="K40" s="2">
         <v>45697.77134046296</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
         <v>33</v>
@@ -1931,30 +1955,30 @@
         <v>49</v>
       </c>
       <c r="F41" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G41" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H41" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I41" t="s">
-        <v>71</v>
-      </c>
-      <c r="L41" s="2">
+        <v>79</v>
+      </c>
+      <c r="J41" s="2">
         <v>45697.80391393518</v>
       </c>
-      <c r="M41" s="2">
+      <c r="K41" s="2">
         <v>45697.80391412037</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C42" t="s">
         <v>33</v>
@@ -1966,30 +1990,30 @@
         <v>47</v>
       </c>
       <c r="F42" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G42" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H42" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I42" t="s">
-        <v>71</v>
-      </c>
-      <c r="L42" s="2">
+        <v>79</v>
+      </c>
+      <c r="J42" s="2">
         <v>45697.94781789352</v>
       </c>
-      <c r="M42" s="2">
+      <c r="K42" s="2">
         <v>45697.94781789352</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C43" t="s">
         <v>33</v>
@@ -2001,30 +2025,30 @@
         <v>47</v>
       </c>
       <c r="F43" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G43" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H43" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I43" t="s">
-        <v>71</v>
-      </c>
-      <c r="L43" s="2">
+        <v>79</v>
+      </c>
+      <c r="J43" s="2">
         <v>45697.9507206713</v>
       </c>
-      <c r="M43" s="2">
+      <c r="K43" s="2">
         <v>45697.9507206713</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C44" t="s">
         <v>33</v>
@@ -2036,30 +2060,30 @@
         <v>47</v>
       </c>
       <c r="F44" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G44" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H44" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I44" t="s">
-        <v>71</v>
-      </c>
-      <c r="L44" s="2">
+        <v>79</v>
+      </c>
+      <c r="J44" s="2">
         <v>45697.95630715278</v>
       </c>
-      <c r="M44" s="2">
+      <c r="K44" s="2">
         <v>45697.95630863426</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C45" t="s">
         <v>33</v>
@@ -2071,30 +2095,30 @@
         <v>47</v>
       </c>
       <c r="F45" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G45" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H45" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I45" t="s">
-        <v>71</v>
-      </c>
-      <c r="L45" s="2">
+        <v>79</v>
+      </c>
+      <c r="J45" s="2">
         <v>45697.96365546296</v>
       </c>
-      <c r="M45" s="2">
+      <c r="K45" s="2">
         <v>45697.96365547454</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C46" t="s">
         <v>33</v>
@@ -2106,30 +2130,30 @@
         <v>47</v>
       </c>
       <c r="F46" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G46" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H46" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I46" t="s">
-        <v>71</v>
-      </c>
-      <c r="L46" s="2">
+        <v>79</v>
+      </c>
+      <c r="J46" s="2">
         <v>45697.96605730324</v>
       </c>
-      <c r="M46" s="2">
+      <c r="K46" s="2">
         <v>45697.96605730324</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C47" t="s">
         <v>33</v>
@@ -2141,30 +2165,30 @@
         <v>47</v>
       </c>
       <c r="F47" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G47" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H47" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I47" t="s">
-        <v>71</v>
-      </c>
-      <c r="L47" s="2">
+        <v>79</v>
+      </c>
+      <c r="J47" s="2">
         <v>45697.97545526621</v>
       </c>
-      <c r="M47" s="2">
+      <c r="K47" s="2">
         <v>45697.97545527778</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C48" t="s">
         <v>33</v>
@@ -2176,30 +2200,30 @@
         <v>47</v>
       </c>
       <c r="F48" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G48" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H48" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I48" t="s">
-        <v>71</v>
-      </c>
-      <c r="L48" s="2">
+        <v>79</v>
+      </c>
+      <c r="J48" s="2">
         <v>45697.97682180555</v>
       </c>
-      <c r="M48" s="2">
+      <c r="K48" s="2">
         <v>45697.97682180555</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:11">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C49" t="s">
         <v>33</v>
@@ -2211,30 +2235,30 @@
         <v>47</v>
       </c>
       <c r="F49" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G49" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H49" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I49" t="s">
-        <v>71</v>
-      </c>
-      <c r="L49" s="2">
+        <v>79</v>
+      </c>
+      <c r="J49" s="2">
         <v>45697.98043483796</v>
       </c>
-      <c r="M49" s="2">
+      <c r="K49" s="2">
         <v>45697.98043483796</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:11">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C50" t="s">
         <v>33</v>
@@ -2246,30 +2270,30 @@
         <v>47</v>
       </c>
       <c r="F50" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G50" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H50" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I50" t="s">
-        <v>71</v>
-      </c>
-      <c r="L50" s="2">
+        <v>79</v>
+      </c>
+      <c r="J50" s="2">
         <v>45697.98127917824</v>
       </c>
-      <c r="M50" s="2">
+      <c r="K50" s="2">
         <v>45697.98127917824</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:11">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C51" t="s">
         <v>35</v>
@@ -2281,30 +2305,30 @@
         <v>47</v>
       </c>
       <c r="F51" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G51" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H51" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I51" t="s">
-        <v>71</v>
-      </c>
-      <c r="L51" s="2">
+        <v>79</v>
+      </c>
+      <c r="J51" s="2">
         <v>45697.98519137732</v>
       </c>
-      <c r="M51" s="2">
+      <c r="K51" s="2">
         <v>45697.98519137732</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:11">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
         <v>35</v>
@@ -2316,30 +2340,30 @@
         <v>47</v>
       </c>
       <c r="F52" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="G52" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H52" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I52" t="s">
-        <v>71</v>
-      </c>
-      <c r="L52" s="2">
+        <v>79</v>
+      </c>
+      <c r="J52" s="2">
         <v>45697.98736938657</v>
       </c>
-      <c r="M52" s="2">
+      <c r="K52" s="2">
         <v>45697.98736940972</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:11">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s">
         <v>33</v>
@@ -2351,30 +2375,30 @@
         <v>42</v>
       </c>
       <c r="F53" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G53" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="H53" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="I53" t="s">
-        <v>71</v>
-      </c>
-      <c r="L53" s="2">
-        <v>45697.99815845337</v>
-      </c>
-      <c r="M53" s="2">
-        <v>45697.99815863415</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
+        <v>79</v>
+      </c>
+      <c r="J53" s="2">
+        <v>45697.99815844907</v>
+      </c>
+      <c r="K53" s="2">
+        <v>45697.99815863426</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C54" t="s">
         <v>35</v>
@@ -2386,22 +2410,477 @@
         <v>43</v>
       </c>
       <c r="F54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G54" t="s">
+        <v>66</v>
+      </c>
+      <c r="H54" t="s">
+        <v>77</v>
+      </c>
+      <c r="I54" t="s">
+        <v>80</v>
+      </c>
+      <c r="J54" s="2">
+        <v>45697.99830934028</v>
+      </c>
+      <c r="K54" s="2">
+        <v>45697.99830934028</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" t="s">
+        <v>62</v>
+      </c>
+      <c r="G55" t="s">
+        <v>71</v>
+      </c>
+      <c r="H55" t="s">
+        <v>78</v>
+      </c>
+      <c r="I55" t="s">
+        <v>79</v>
+      </c>
+      <c r="J55" s="2">
+        <v>45698.02574974537</v>
+      </c>
+      <c r="K55" s="2">
+        <v>45698.02574975695</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+      <c r="D56" t="s">
+        <v>37</v>
+      </c>
+      <c r="E56" t="s">
+        <v>50</v>
+      </c>
+      <c r="F56" t="s">
+        <v>62</v>
+      </c>
+      <c r="G56" t="s">
+        <v>71</v>
+      </c>
+      <c r="H56" t="s">
+        <v>78</v>
+      </c>
+      <c r="I56" t="s">
+        <v>79</v>
+      </c>
+      <c r="J56" s="2">
+        <v>45698.02700150463</v>
+      </c>
+      <c r="K56" s="2">
+        <v>45698.02700150463</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>31</v>
+      </c>
+      <c r="C57" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" t="s">
+        <v>62</v>
+      </c>
+      <c r="G57" t="s">
+        <v>71</v>
+      </c>
+      <c r="H57" t="s">
+        <v>78</v>
+      </c>
+      <c r="I57" t="s">
+        <v>79</v>
+      </c>
+      <c r="J57" s="2">
+        <v>45698.03398265046</v>
+      </c>
+      <c r="K57" s="2">
+        <v>45698.03398266204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" t="s">
+        <v>37</v>
+      </c>
+      <c r="E58" t="s">
+        <v>50</v>
+      </c>
+      <c r="F58" t="s">
+        <v>62</v>
+      </c>
+      <c r="G58" t="s">
+        <v>71</v>
+      </c>
+      <c r="H58" t="s">
+        <v>78</v>
+      </c>
+      <c r="I58" t="s">
+        <v>79</v>
+      </c>
+      <c r="J58" s="2">
+        <v>45698.03442172454</v>
+      </c>
+      <c r="K58" s="2">
+        <v>45698.03442172454</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" t="s">
+        <v>37</v>
+      </c>
+      <c r="E59" t="s">
         <v>51</v>
       </c>
-      <c r="G54" t="s">
+      <c r="F59" t="s">
+        <v>63</v>
+      </c>
+      <c r="G59" t="s">
+        <v>71</v>
+      </c>
+      <c r="H59" t="s">
+        <v>74</v>
+      </c>
+      <c r="I59" t="s">
+        <v>81</v>
+      </c>
+      <c r="J59" s="2">
+        <v>45698.06702224537</v>
+      </c>
+      <c r="K59" s="2">
+        <v>45698.06702224537</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" t="s">
+        <v>34</v>
+      </c>
+      <c r="D60" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" t="s">
+        <v>51</v>
+      </c>
+      <c r="F60" t="s">
+        <v>63</v>
+      </c>
+      <c r="G60" t="s">
+        <v>71</v>
+      </c>
+      <c r="H60" t="s">
+        <v>74</v>
+      </c>
+      <c r="I60" t="s">
+        <v>81</v>
+      </c>
+      <c r="J60" s="2">
+        <v>45698.06803696759</v>
+      </c>
+      <c r="K60" s="2">
+        <v>45698.06803696759</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61">
         <v>60</v>
       </c>
-      <c r="H54" t="s">
-        <v>70</v>
-      </c>
-      <c r="I54" t="s">
-        <v>72</v>
-      </c>
-      <c r="L54" s="2">
-        <v>45697.99830934116</v>
-      </c>
-      <c r="M54" s="2">
-        <v>45697.99830934116</v>
+      <c r="B61" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" t="s">
+        <v>34</v>
+      </c>
+      <c r="D61" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" t="s">
+        <v>63</v>
+      </c>
+      <c r="G61" t="s">
+        <v>71</v>
+      </c>
+      <c r="H61" t="s">
+        <v>74</v>
+      </c>
+      <c r="I61" t="s">
+        <v>81</v>
+      </c>
+      <c r="J61" s="2">
+        <v>45698.06938768519</v>
+      </c>
+      <c r="K61" s="2">
+        <v>45698.06938768519</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" t="s">
+        <v>34</v>
+      </c>
+      <c r="D62" t="s">
+        <v>37</v>
+      </c>
+      <c r="E62" t="s">
+        <v>51</v>
+      </c>
+      <c r="F62" t="s">
+        <v>63</v>
+      </c>
+      <c r="G62" t="s">
+        <v>71</v>
+      </c>
+      <c r="H62" t="s">
+        <v>74</v>
+      </c>
+      <c r="I62" t="s">
+        <v>81</v>
+      </c>
+      <c r="J62" s="2">
+        <v>45698.07060145833</v>
+      </c>
+      <c r="K62" s="2">
+        <v>45698.07060145833</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" t="s">
+        <v>34</v>
+      </c>
+      <c r="D63" t="s">
+        <v>37</v>
+      </c>
+      <c r="E63" t="s">
+        <v>51</v>
+      </c>
+      <c r="F63" t="s">
+        <v>63</v>
+      </c>
+      <c r="G63" t="s">
+        <v>71</v>
+      </c>
+      <c r="H63" t="s">
+        <v>74</v>
+      </c>
+      <c r="I63" t="s">
+        <v>81</v>
+      </c>
+      <c r="J63" s="2">
+        <v>45698.07605251158</v>
+      </c>
+      <c r="K63" s="2">
+        <v>45698.07605251158</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" t="s">
+        <v>33</v>
+      </c>
+      <c r="D64" t="s">
+        <v>37</v>
+      </c>
+      <c r="E64" t="s">
+        <v>42</v>
+      </c>
+      <c r="F64" t="s">
+        <v>53</v>
+      </c>
+      <c r="G64" t="s">
+        <v>65</v>
+      </c>
+      <c r="H64" t="s">
+        <v>72</v>
+      </c>
+      <c r="I64" t="s">
+        <v>79</v>
+      </c>
+      <c r="J64" s="2">
+        <v>45698.08615400463</v>
+      </c>
+      <c r="K64" s="2">
+        <v>45698.0861540162</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" t="s">
+        <v>39</v>
+      </c>
+      <c r="E65" t="s">
+        <v>43</v>
+      </c>
+      <c r="F65" t="s">
+        <v>54</v>
+      </c>
+      <c r="G65" t="s">
+        <v>66</v>
+      </c>
+      <c r="H65" t="s">
+        <v>77</v>
+      </c>
+      <c r="I65" t="s">
+        <v>80</v>
+      </c>
+      <c r="J65" s="2">
+        <v>45698.08627409722</v>
+      </c>
+      <c r="K65" s="2">
+        <v>45698.0862741088</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>32</v>
+      </c>
+      <c r="C66" t="s">
+        <v>34</v>
+      </c>
+      <c r="D66" t="s">
+        <v>37</v>
+      </c>
+      <c r="E66" t="s">
+        <v>51</v>
+      </c>
+      <c r="F66" t="s">
+        <v>63</v>
+      </c>
+      <c r="G66" t="s">
+        <v>71</v>
+      </c>
+      <c r="H66" t="s">
+        <v>74</v>
+      </c>
+      <c r="I66" t="s">
+        <v>81</v>
+      </c>
+      <c r="J66" s="2">
+        <v>45698.10421476852</v>
+      </c>
+      <c r="K66" s="2">
+        <v>45698.10421476852</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>20</v>
+      </c>
+      <c r="C67" t="s">
+        <v>33</v>
+      </c>
+      <c r="D67" t="s">
+        <v>39</v>
+      </c>
+      <c r="E67" t="s">
+        <v>52</v>
+      </c>
+      <c r="F67" t="s">
+        <v>64</v>
+      </c>
+      <c r="G67" t="s">
+        <v>71</v>
+      </c>
+      <c r="H67" t="s">
+        <v>76</v>
+      </c>
+      <c r="I67" t="s">
+        <v>82</v>
+      </c>
+      <c r="J67" s="2">
+        <v>45698.12894751628</v>
+      </c>
+      <c r="K67" s="2">
+        <v>45698.12894751628</v>
       </c>
     </row>
   </sheetData>
@@ -2411,7 +2890,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2422,10 +2901,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2433,10 +2912,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2444,10 +2923,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2455,10 +2934,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2466,10 +2945,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2477,10 +2956,10 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2488,10 +2967,10 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2499,10 +2978,10 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2510,10 +2989,10 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2521,10 +3000,10 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2532,10 +3011,10 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2543,10 +3022,10 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2554,10 +3033,10 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2565,10 +3044,10 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2576,10 +3055,10 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2597,10 +3076,10 @@
         <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2608,10 +3087,10 @@
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2619,10 +3098,10 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2630,10 +3109,10 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2641,10 +3120,10 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2652,10 +3131,10 @@
         <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2663,10 +3142,10 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2674,10 +3153,10 @@
         <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2685,10 +3164,10 @@
         <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2696,10 +3175,10 @@
         <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2707,10 +3186,10 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2718,10 +3197,10 @@
         <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2729,10 +3208,10 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2740,10 +3219,10 @@
         <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2751,10 +3230,10 @@
         <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2762,10 +3241,10 @@
         <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2773,10 +3252,10 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2784,10 +3263,10 @@
         <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2795,10 +3274,10 @@
         <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2806,10 +3285,10 @@
         <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2817,10 +3296,10 @@
         <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2828,10 +3307,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2839,10 +3318,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C40" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2850,10 +3329,10 @@
         <v>48</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2861,10 +3340,10 @@
         <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2872,10 +3351,10 @@
         <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2883,10 +3362,10 @@
         <v>51</v>
       </c>
       <c r="B44" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2894,10 +3373,10 @@
         <v>52</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2905,10 +3384,10 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2916,10 +3395,10 @@
         <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2927,10 +3406,10 @@
         <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2938,10 +3417,10 @@
         <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2949,10 +3428,10 @@
         <v>57</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2960,10 +3439,10 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2971,10 +3450,186 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C52" t="s">
-        <v>78</v>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54">
+        <v>55</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55">
+        <v>56</v>
+      </c>
+      <c r="B55" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56">
+        <v>57</v>
+      </c>
+      <c r="B56" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57">
+        <v>2</v>
+      </c>
+      <c r="B57" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>87</v>
+      </c>
+      <c r="C58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63">
+        <v>25</v>
+      </c>
+      <c r="B63" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67">
+        <v>16</v>
+      </c>
+      <c r="B67" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>85</v>
+      </c>
+      <c r="C68" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>